<commit_message>
Cafesito por la mañana
Actualizaciones
</commit_message>
<xml_diff>
--- a/appGAS - Gestion/CR_CronogramaResponsabilidades/CR_CronogramaResponsabilidades.xlsx
+++ b/appGAS - Gestion/CR_CronogramaResponsabilidades/CR_CronogramaResponsabilidades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angel\Desktop\gasAPP\aplicacionesMOB_cc75\appGAS - Gestion\CR_CronogramaResponsabilidades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2397F0AB-E7B1-444E-AE3D-90C06BB1D3F8}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF50C23B-5BEA-46CC-933E-E69351466FB1}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{03FCA750-3069-4E98-8889-EDFFACBD7BA7}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_Custodio">Hoja1!$A$34:$A$38</definedName>
-    <definedName name="_Estado">Hoja1!$B$34:$B$39</definedName>
+    <definedName name="_Custodio">Hoja1!$A$37:$A$41</definedName>
+    <definedName name="_Estado">Hoja1!$B$37:$B$42</definedName>
   </definedNames>
   <calcPr calcId="179017"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="43">
   <si>
     <t>Fecha Inicio</t>
   </si>
@@ -144,6 +144,25 @@
   <si>
     <t>REVISAR WBS PROYECTO Y APLICACIÓN
 REVISAR COMENTARIOS EN EL DOCUMENTO</t>
+  </si>
+  <si>
+    <t>RESUELTO</t>
+  </si>
+  <si>
+    <t>C:\Users\angel\Desktop\gasAPP\aplicacionesMOB_cc75\appGAS - Analisis\UML_CasosdeUso
+C:\Users\angel\Desktop\gasAPP\aplicacionesMOB_cc75\appGAS - Analisis\ECU_EspecificacionCasosDeUso
+C:\Users\angel\Desktop\gasAPP\aplicacionesMOB_cc75\appGAS - PlanDeDesarrollo\PS_PlanificacionScrum</t>
+  </si>
+  <si>
+    <t>Casos de uso - CAPITULO 3
++SCRUM</t>
+  </si>
+  <si>
+    <t>Resumen de tecnologías aplicadas en el diseño y desarrollo de la solución
+IGUAL A VISTA DESPLIEGUE</t>
+  </si>
+  <si>
+    <t>C:\Users\angel\Desktop\gasAPP\aplicacionesMOB_cc75\appGAS - Diseno\VD_VistaDespliegue</t>
   </si>
 </sst>
 </file>
@@ -317,7 +336,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -341,102 +360,25 @@
     <xf numFmtId="14" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="16">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -907,15 +849,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD9EF44E-C7EE-447A-A024-D7352D22FCC0}">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="46" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="63.5703125" customWidth="1"/>
+    <col min="1" max="1" width="73.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="52" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="123.5703125" bestFit="1" customWidth="1"/>
@@ -959,10 +901,10 @@
       <c r="C2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="23"/>
+      <c r="E2" s="21"/>
       <c r="F2" s="11">
         <v>43223</v>
       </c>
@@ -989,7 +931,7 @@
         <v>43223</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>24</v>
       </c>
@@ -1002,8 +944,8 @@
       <c r="D4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="24" t="s">
-        <v>37</v>
+      <c r="E4" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="F4" s="11">
         <v>43224</v>
@@ -1012,7 +954,7 @@
         <v>43224</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>25</v>
       </c>
@@ -1025,8 +967,8 @@
       <c r="D5" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="24" t="s">
-        <v>37</v>
+      <c r="E5" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="F5" s="11">
         <v>43224</v>
@@ -1098,9 +1040,9 @@
         <v>43224</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>29</v>
+    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="23" t="s">
+        <v>40</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>8</v>
@@ -1108,12 +1050,10 @@
       <c r="C9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="24" t="s">
-        <v>37</v>
-      </c>
+      <c r="D9" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="3"/>
       <c r="F9" s="11">
         <v>43224</v>
       </c>
@@ -1121,271 +1061,320 @@
         <v>43224</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5" t="s">
-        <v>4</v>
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
+      <c r="D10" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5" t="s">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+    </row>
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" s="11">
+        <v>43224</v>
+      </c>
+      <c r="G12" s="11">
+        <v>43224</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5" t="s">
         <v>4</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6" t="s">
-        <v>5</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7" t="s">
-        <v>6</v>
+      <c r="A14" s="5"/>
+      <c r="B14" s="5" t="s">
+        <v>4</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7" t="s">
-        <v>6</v>
+      <c r="A15" s="6"/>
+      <c r="B15" s="6" t="s">
+        <v>5</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8" t="s">
-        <v>7</v>
+      <c r="A16" s="6"/>
+      <c r="B16" s="6" t="s">
+        <v>5</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8" t="s">
-        <v>7</v>
+      <c r="A17" s="7"/>
+      <c r="B17" s="7" t="s">
+        <v>6</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="20"/>
-    </row>
-    <row r="20" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="7"/>
+      <c r="B18" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="8"/>
+      <c r="B19" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="8"/>
+      <c r="B20" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+    </row>
+    <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="11">
+      <c r="B23" s="11">
         <v>43223</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
+    <row r="24" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B24" s="12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="21" t="s">
+    <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="22"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="15" t="s">
+      <c r="B26" s="25"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="15" t="s">
+      <c r="B27" s="15" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="16">
-        <v>1</v>
-      </c>
-      <c r="B25" s="13"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="16">
-        <v>2</v>
-      </c>
-      <c r="B26" s="2"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="16">
-        <v>3</v>
-      </c>
-      <c r="B27" s="14"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="16">
+        <v>1</v>
+      </c>
+      <c r="B28" s="13"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="16">
+        <v>2</v>
+      </c>
+      <c r="B29" s="2"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="16">
+        <v>3</v>
+      </c>
+      <c r="B30" s="14"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="16">
         <v>4</v>
       </c>
-      <c r="B28" s="4"/>
-    </row>
-    <row r="34" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>8</v>
-      </c>
-      <c r="B34" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>4</v>
-      </c>
-      <c r="B35" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>5</v>
-      </c>
-      <c r="B36" t="s">
-        <v>11</v>
-      </c>
+      <c r="B31" s="4"/>
     </row>
     <row r="37" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B37" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="38" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>6</v>
+      </c>
+      <c r="B40" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>7</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B41" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
+    <row r="42" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="40" spans="1:2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:2" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A26:B26"/>
   </mergeCells>
-  <conditionalFormatting sqref="C10:C17 C2:C8">
-    <cfRule type="containsText" dxfId="23" priority="17" operator="containsText" text="TRANSFERIDO">
+  <conditionalFormatting sqref="C13:C20 C2:C11">
+    <cfRule type="containsText" dxfId="15" priority="17" operator="containsText" text="TRANSFERIDO">
       <formula>NOT(ISERROR(SEARCH("TRANSFERIDO",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="18" operator="containsText" text="PROCESO">
+    <cfRule type="containsText" dxfId="14" priority="18" operator="containsText" text="PROCESO">
       <formula>NOT(ISERROR(SEARCH("PROCESO",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="19" operator="containsText" text="POR HACER">
+    <cfRule type="containsText" dxfId="13" priority="19" operator="containsText" text="POR HACER">
       <formula>NOT(ISERROR(SEARCH("POR HACER",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="20" operator="containsText" text="POR HACER">
+    <cfRule type="containsText" dxfId="12" priority="20" operator="containsText" text="POR HACER">
       <formula>NOT(ISERROR(SEARCH("POR HACER",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="21" operator="containsText" text="PAUSADO">
+    <cfRule type="containsText" dxfId="11" priority="21" operator="containsText" text="PAUSADO">
       <formula>NOT(ISERROR(SEARCH("PAUSADO",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="22" operator="containsText" text="POR HACER">
+    <cfRule type="containsText" dxfId="10" priority="22" operator="containsText" text="POR HACER">
       <formula>NOT(ISERROR(SEARCH("POR HACER",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="23" operator="containsText" text="SEGUIMIENTO">
+    <cfRule type="containsText" dxfId="9" priority="23" operator="containsText" text="SEGUIMIENTO">
       <formula>NOT(ISERROR(SEARCH("SEGUIMIENTO",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="24" operator="containsText" text="FINALIZADO">
+    <cfRule type="containsText" dxfId="8" priority="24" operator="containsText" text="FINALIZADO">
       <formula>NOT(ISERROR(SEARCH("FINALIZADO",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C9">
-    <cfRule type="containsText" dxfId="15" priority="1" operator="containsText" text="TRANSFERIDO">
-      <formula>NOT(ISERROR(SEARCH("TRANSFERIDO",C9)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="2" operator="containsText" text="PROCESO">
-      <formula>NOT(ISERROR(SEARCH("PROCESO",C9)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="3" operator="containsText" text="POR HACER">
-      <formula>NOT(ISERROR(SEARCH("POR HACER",C9)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="4" operator="containsText" text="POR HACER">
-      <formula>NOT(ISERROR(SEARCH("POR HACER",C9)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="5" operator="containsText" text="PAUSADO">
-      <formula>NOT(ISERROR(SEARCH("PAUSADO",C9)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="6" operator="containsText" text="POR HACER">
-      <formula>NOT(ISERROR(SEARCH("POR HACER",C9)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="7" operator="containsText" text="SEGUIMIENTO">
-      <formula>NOT(ISERROR(SEARCH("SEGUIMIENTO",C9)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="8" operator="containsText" text="FINALIZADO">
-      <formula>NOT(ISERROR(SEARCH("FINALIZADO",C9)))</formula>
+  <conditionalFormatting sqref="C12">
+    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="TRANSFERIDO">
+      <formula>NOT(ISERROR(SEARCH("TRANSFERIDO",C12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="PROCESO">
+      <formula>NOT(ISERROR(SEARCH("PROCESO",C12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="POR HACER">
+      <formula>NOT(ISERROR(SEARCH("POR HACER",C12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="POR HACER">
+      <formula>NOT(ISERROR(SEARCH("POR HACER",C12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="PAUSADO">
+      <formula>NOT(ISERROR(SEARCH("PAUSADO",C12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="6" operator="containsText" text="POR HACER">
+      <formula>NOT(ISERROR(SEARCH("POR HACER",C12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="7" operator="containsText" text="SEGUIMIENTO">
+      <formula>NOT(ISERROR(SEARCH("SEGUIMIENTO",C12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="8" operator="containsText" text="FINALIZADO">
+      <formula>NOT(ISERROR(SEARCH("FINALIZADO",C12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10:B17 B2:B8" xr:uid="{7F479649-180B-44B5-940B-62A43F3A2E18}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:B20 B2:B11" xr:uid="{7F479649-180B-44B5-940B-62A43F3A2E18}">
       <formula1>_Custodio</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C17" xr:uid="{2F4C52C3-C722-4F93-B140-536C40737886}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C20" xr:uid="{2F4C52C3-C722-4F93-B140-536C40737886}">
       <formula1>_Estado</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Cervecita por la madrugrada
Nuevos documentos
</commit_message>
<xml_diff>
--- a/appGAS - Gestion/CR_CronogramaResponsabilidades/CR_CronogramaResponsabilidades.xlsx
+++ b/appGAS - Gestion/CR_CronogramaResponsabilidades/CR_CronogramaResponsabilidades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angel\Desktop\gasAPP\aplicacionesMOB_cc75\appGAS - Gestion\CR_CronogramaResponsabilidades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF50C23B-5BEA-46CC-933E-E69351466FB1}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB2B635B-EB72-4E44-B8B4-7866FA7B32BB}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{03FCA750-3069-4E98-8889-EDFFACBD7BA7}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_Custodio">Hoja1!$A$37:$A$41</definedName>
-    <definedName name="_Estado">Hoja1!$B$37:$B$42</definedName>
+    <definedName name="_Custodio">Hoja1!$A$38:$A$42</definedName>
+    <definedName name="_Estado">Hoja1!$B$38:$B$43</definedName>
   </definedNames>
   <calcPr calcId="179017"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="47">
   <si>
     <t>Fecha Inicio</t>
   </si>
@@ -163,6 +163,18 @@
   </si>
   <si>
     <t>C:\Users\angel\Desktop\gasAPP\aplicacionesMOB_cc75\appGAS - Diseno\VD_VistaDespliegue</t>
+  </si>
+  <si>
+    <t>Documento de Stakeholders</t>
+  </si>
+  <si>
+    <t>C:\Users\angel\Desktop\gasAPP\aplicacionesMOB_cc75\appGAS - Analisis\STH_StakeHolders</t>
+  </si>
+  <si>
+    <t>Documento Esquema de Repositorios</t>
+  </si>
+  <si>
+    <t>C:\Users\angel\Desktop\gasAPP\aplicacionesMOB_cc75\appGAS - Gestion\PGC_PlanDeGestionDeConfiguracion\EI_EsquemaDeRepositorio</t>
   </si>
 </sst>
 </file>
@@ -849,10 +861,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD9EF44E-C7EE-447A-A024-D7352D22FCC0}">
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -860,7 +872,7 @@
     <col min="1" max="1" width="73.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="52" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="123.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="139.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="113.42578125" customWidth="1"/>
     <col min="6" max="6" width="17.42578125" style="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.7109375" style="9" bestFit="1" customWidth="1"/>
@@ -1075,21 +1087,37 @@
         <v>42</v>
       </c>
       <c r="E10" s="3"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
+      <c r="F10" s="11">
+        <v>43224</v>
+      </c>
+      <c r="G10" s="11">
+        <v>43224</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
+      <c r="A11" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="E11" s="3"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-    </row>
-    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="F11" s="11">
+        <v>43224</v>
+      </c>
+      <c r="G11" s="11">
+        <v>43224</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>8</v>
@@ -1098,30 +1126,34 @@
         <v>9</v>
       </c>
       <c r="D12" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" s="3"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+    </row>
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="22" t="s">
+      <c r="E13" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="F12" s="11">
-        <v>43224</v>
-      </c>
-      <c r="G12" s="11">
-        <v>43224</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
+      <c r="F13" s="11">
+        <v>43224</v>
+      </c>
+      <c r="G13" s="11">
+        <v>43224</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
@@ -1137,17 +1169,17 @@
       <c r="G14" s="17"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6" t="s">
-        <v>5</v>
+      <c r="A15" s="5"/>
+      <c r="B15" s="5" t="s">
+        <v>4</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
@@ -1163,17 +1195,17 @@
       <c r="G16" s="18"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7" t="s">
-        <v>6</v>
+      <c r="A17" s="6"/>
+      <c r="B17" s="6" t="s">
+        <v>5</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
@@ -1189,17 +1221,17 @@
       <c r="G18" s="19"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8" t="s">
-        <v>7</v>
+      <c r="A19" s="7"/>
+      <c r="B19" s="7" t="s">
+        <v>6</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
@@ -1214,111 +1246,124 @@
       <c r="F20" s="20"/>
       <c r="G20" s="20"/>
     </row>
-    <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B23" s="11">
-        <v>43223</v>
-      </c>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="8"/>
+      <c r="B21" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
     </row>
     <row r="24" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" s="11">
+        <v>43223</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B25" s="12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="24" t="s">
+    <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="B26" s="25"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="15" t="s">
+      <c r="B27" s="25"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B28" s="15" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="16">
-        <v>1</v>
-      </c>
-      <c r="B28" s="13"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="16">
-        <v>2</v>
-      </c>
-      <c r="B29" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="B29" s="13"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="16">
-        <v>3</v>
-      </c>
-      <c r="B30" s="14"/>
+        <v>2</v>
+      </c>
+      <c r="B30" s="2"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="16">
+        <v>3</v>
+      </c>
+      <c r="B31" s="14"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="16">
         <v>4</v>
       </c>
-      <c r="B31" s="4"/>
-    </row>
-    <row r="37" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>8</v>
-      </c>
-      <c r="B37" t="s">
-        <v>9</v>
-      </c>
+      <c r="B32" s="4"/>
     </row>
     <row r="38" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B38" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="39" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B39" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B40" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="41" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>6</v>
+      </c>
+      <c r="B41" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>7</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
+    <row r="43" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="43" spans="1:2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:2" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
   </mergeCells>
-  <conditionalFormatting sqref="C13:C20 C2:C11">
+  <conditionalFormatting sqref="C14:C21 C2:C12">
     <cfRule type="containsText" dxfId="15" priority="17" operator="containsText" text="TRANSFERIDO">
       <formula>NOT(ISERROR(SEARCH("TRANSFERIDO",C2)))</formula>
     </cfRule>
@@ -1344,37 +1389,37 @@
       <formula>NOT(ISERROR(SEARCH("FINALIZADO",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C12">
+  <conditionalFormatting sqref="C13">
     <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="TRANSFERIDO">
-      <formula>NOT(ISERROR(SEARCH("TRANSFERIDO",C12)))</formula>
+      <formula>NOT(ISERROR(SEARCH("TRANSFERIDO",C13)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="PROCESO">
-      <formula>NOT(ISERROR(SEARCH("PROCESO",C12)))</formula>
+      <formula>NOT(ISERROR(SEARCH("PROCESO",C13)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="POR HACER">
-      <formula>NOT(ISERROR(SEARCH("POR HACER",C12)))</formula>
+      <formula>NOT(ISERROR(SEARCH("POR HACER",C13)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="POR HACER">
-      <formula>NOT(ISERROR(SEARCH("POR HACER",C12)))</formula>
+      <formula>NOT(ISERROR(SEARCH("POR HACER",C13)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="PAUSADO">
-      <formula>NOT(ISERROR(SEARCH("PAUSADO",C12)))</formula>
+      <formula>NOT(ISERROR(SEARCH("PAUSADO",C13)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="2" priority="6" operator="containsText" text="POR HACER">
-      <formula>NOT(ISERROR(SEARCH("POR HACER",C12)))</formula>
+      <formula>NOT(ISERROR(SEARCH("POR HACER",C13)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="1" priority="7" operator="containsText" text="SEGUIMIENTO">
-      <formula>NOT(ISERROR(SEARCH("SEGUIMIENTO",C12)))</formula>
+      <formula>NOT(ISERROR(SEARCH("SEGUIMIENTO",C13)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="0" priority="8" operator="containsText" text="FINALIZADO">
-      <formula>NOT(ISERROR(SEARCH("FINALIZADO",C12)))</formula>
+      <formula>NOT(ISERROR(SEARCH("FINALIZADO",C13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:B20 B2:B11" xr:uid="{7F479649-180B-44B5-940B-62A43F3A2E18}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B14:B21 B2:B12" xr:uid="{7F479649-180B-44B5-940B-62A43F3A2E18}">
       <formula1>_Custodio</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C20" xr:uid="{2F4C52C3-C722-4F93-B140-536C40737886}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C21" xr:uid="{2F4C52C3-C722-4F93-B140-536C40737886}">
       <formula1>_Estado</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>